<commit_message>
updated frontend and backend
</commit_message>
<xml_diff>
--- a/backend/backend/data.xlsx
+++ b/backend/backend/data.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -420,7 +420,31 @@
         <v>accountNumber</v>
       </c>
       <c r="E1" t="str">
-        <v>timestamp</v>
+        <v>Date and Time</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Project Id</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Account number</v>
+      </c>
+      <c r="I1" t="str">
+        <v>PO number</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Vendor Name</v>
+      </c>
+      <c r="K1" t="str">
+        <v>IFSC code</v>
+      </c>
+      <c r="L1" t="str">
+        <v>status</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Remarks</v>
       </c>
     </row>
     <row r="2">
@@ -479,9 +503,124 @@
         <v xml:space="preserve">565 </v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>test009</v>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve">854 </v>
+      </c>
+      <c r="C6" t="str">
+        <v xml:space="preserve">gowtham </v>
+      </c>
+      <c r="D6" t="str">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">test009 </v>
+      </c>
+      <c r="B7" t="str">
+        <v xml:space="preserve">854 </v>
+      </c>
+      <c r="C7" t="str">
+        <v xml:space="preserve">tester </v>
+      </c>
+      <c r="D7" t="str">
+        <v xml:space="preserve">777888 </v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="E8" t="str">
+        <v>09-10-2024</v>
+      </c>
+      <c r="F8" t="str">
+        <v xml:space="preserve">00 </v>
+      </c>
+      <c r="G8" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H8" t="str">
+        <v xml:space="preserve">777888 </v>
+      </c>
+      <c r="I8" t="str">
+        <v xml:space="preserve">33 </v>
+      </c>
+      <c r="J8" t="str">
+        <v xml:space="preserve">tester </v>
+      </c>
+      <c r="K8" t="str">
+        <v>test007</v>
+      </c>
+      <c r="L8" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M8" t="str">
+        <v>Testing Reason</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="E9" t="str">
+        <v>09-10-2024</v>
+      </c>
+      <c r="F9" t="str">
+        <v>100000</v>
+      </c>
+      <c r="G9" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H9" t="str">
+        <v xml:space="preserve">777888 </v>
+      </c>
+      <c r="I9" t="str">
+        <v>g</v>
+      </c>
+      <c r="J9" t="str">
+        <v xml:space="preserve">tester </v>
+      </c>
+      <c r="K9" t="str">
+        <v>test007</v>
+      </c>
+      <c r="L9" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M9" t="str">
+        <v>Testing Reason</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="E10" t="str">
+        <v>09-10-2024</v>
+      </c>
+      <c r="F10" t="str">
+        <v>00</v>
+      </c>
+      <c r="G10" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H10" t="str">
+        <v>696</v>
+      </c>
+      <c r="I10" t="str">
+        <v xml:space="preserve">854 </v>
+      </c>
+      <c r="J10" t="str">
+        <v xml:space="preserve">tester  </v>
+      </c>
+      <c r="K10" t="str">
+        <v>2003</v>
+      </c>
+      <c r="L10" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M10" t="str">
+        <v>Testing Reason</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated status and xl fields
</commit_message>
<xml_diff>
--- a/backend/backend/data.xlsx
+++ b/backend/backend/data.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -676,9 +676,67 @@
         <v>Testing Reason</v>
       </c>
     </row>
+    <row r="13">
+      <c r="E13" t="str">
+        <v>09-10-2024</v>
+      </c>
+      <c r="F13" t="str">
+        <v>345</v>
+      </c>
+      <c r="G13" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H13" t="str">
+        <v>696</v>
+      </c>
+      <c r="I13" t="str">
+        <v>854</v>
+      </c>
+      <c r="J13" t="str">
+        <v xml:space="preserve">gowtham </v>
+      </c>
+      <c r="K13" t="str">
+        <v xml:space="preserve">test009 </v>
+      </c>
+      <c r="L13" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M13" t="str">
+        <v>Other (Entry manually)</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="str">
+        <v>09-10-2024</v>
+      </c>
+      <c r="F14" t="str">
+        <v>345</v>
+      </c>
+      <c r="G14" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H14" t="str">
+        <v xml:space="preserve">777888 </v>
+      </c>
+      <c r="I14" t="str">
+        <v xml:space="preserve">854 </v>
+      </c>
+      <c r="J14" t="str">
+        <v xml:space="preserve">tester  </v>
+      </c>
+      <c r="K14" t="str">
+        <v>90</v>
+      </c>
+      <c r="L14" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M14" t="str">
+        <v>Material schedule No/Service Reason</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added backend for new edit functionality for submitted forms
</commit_message>
<xml_diff>
--- a/backend/backend/data.xlsx
+++ b/backend/backend/data.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -734,9 +734,125 @@
         <v>Material schedule No/Service Reason</v>
       </c>
     </row>
+    <row r="15">
+      <c r="E15" t="str">
+        <v>10-10-2024</v>
+      </c>
+      <c r="F15" t="str">
+        <v xml:space="preserve">345 </v>
+      </c>
+      <c r="G15" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H15" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="I15" t="str">
+        <v xml:space="preserve">854 </v>
+      </c>
+      <c r="J15" t="str">
+        <v>client_deepak</v>
+      </c>
+      <c r="K15" t="str">
+        <v>0987654321</v>
+      </c>
+      <c r="L15" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M15" t="str">
+        <v>Testing Reason</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" t="str">
+        <v>10-10-2024</v>
+      </c>
+      <c r="F16" t="str">
+        <v>9</v>
+      </c>
+      <c r="G16" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H16" t="str">
+        <v>undefined</v>
+      </c>
+      <c r="I16" t="str">
+        <v>undefined</v>
+      </c>
+      <c r="J16" t="str">
+        <v>undefined</v>
+      </c>
+      <c r="K16" t="str">
+        <v>undefined</v>
+      </c>
+      <c r="L16" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M16" t="str">
+        <v>General Reason</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" t="str">
+        <v>10-10-2024</v>
+      </c>
+      <c r="F17" t="str">
+        <v>100</v>
+      </c>
+      <c r="G17" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H17" t="str">
+        <v xml:space="preserve">777888 </v>
+      </c>
+      <c r="I17" t="str">
+        <v xml:space="preserve">33 </v>
+      </c>
+      <c r="J17" t="str">
+        <v>seller</v>
+      </c>
+      <c r="K17" t="str">
+        <v xml:space="preserve">test009 </v>
+      </c>
+      <c r="L17" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M17" t="str">
+        <v>Material schedule No/Service Reason</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" t="str">
+        <v>10-10-2024</v>
+      </c>
+      <c r="F18" t="str">
+        <v>42567</v>
+      </c>
+      <c r="G18" t="str">
+        <v>P23</v>
+      </c>
+      <c r="H18" t="str">
+        <v xml:space="preserve">777888 </v>
+      </c>
+      <c r="I18" t="str">
+        <v>66</v>
+      </c>
+      <c r="J18" t="str">
+        <v>gowtham</v>
+      </c>
+      <c r="K18" t="str">
+        <v xml:space="preserve">test009 </v>
+      </c>
+      <c r="L18" t="str">
+        <v>Submitted</v>
+      </c>
+      <c r="M18" t="str">
+        <v>Testing Reason</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>